<commit_message>
preenchimento aut. juntando textos
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/5.Ferramentas_dados/2.Preenchimento_relampago.xlsx
+++ b/2.Excel/hands-on/5.Ferramentas_dados/2.Preenchimento_relampago.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\5.Ferramentas_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7684AB4-F20C-4657-9F60-6151816AC93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25201E7F-AF5F-43EB-85E4-B3A248AD4BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11112" yWindow="0" windowWidth="11928" windowHeight="12792" activeTab="1" xr2:uid="{F770B815-E08D-404F-8478-C04C9E03FC4D}"/>
+    <workbookView xWindow="11112" yWindow="0" windowWidth="11928" windowHeight="12792" firstSheet="2" activeTab="3" xr2:uid="{F770B815-E08D-404F-8478-C04C9E03FC4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Exemplo1" sheetId="8" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4418" uniqueCount="3292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4828" uniqueCount="3530">
   <si>
     <t>Região</t>
   </si>
@@ -9919,6 +9919,720 @@
   </si>
   <si>
     <t>Uma Noite em Miami</t>
+  </si>
+  <si>
+    <t>São Paulo</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>Brasília</t>
+  </si>
+  <si>
+    <t>Salvador</t>
+  </si>
+  <si>
+    <t>Fortaleza</t>
+  </si>
+  <si>
+    <t>Belo Horizonte</t>
+  </si>
+  <si>
+    <t>Manaus</t>
+  </si>
+  <si>
+    <t>Curitiba</t>
+  </si>
+  <si>
+    <t>Recife</t>
+  </si>
+  <si>
+    <t>Goiânia</t>
+  </si>
+  <si>
+    <t>Belém</t>
+  </si>
+  <si>
+    <t>Porto Alegre</t>
+  </si>
+  <si>
+    <t>Guarulhos</t>
+  </si>
+  <si>
+    <t>Campinas</t>
+  </si>
+  <si>
+    <t>São Luís</t>
+  </si>
+  <si>
+    <t>São Gonçalo</t>
+  </si>
+  <si>
+    <t>Maceió</t>
+  </si>
+  <si>
+    <t>Duque de Caxias</t>
+  </si>
+  <si>
+    <t>Campo Grande</t>
+  </si>
+  <si>
+    <t>Natal</t>
+  </si>
+  <si>
+    <t>Teresina</t>
+  </si>
+  <si>
+    <t>São Bernardo do Campo</t>
+  </si>
+  <si>
+    <t>Nova Iguaçu</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>RJ</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>João Pessoa</t>
+  </si>
+  <si>
+    <t>São José dos Campos</t>
+  </si>
+  <si>
+    <t>Santo André</t>
+  </si>
+  <si>
+    <t>Ribeirão Preto</t>
+  </si>
+  <si>
+    <t>Jaboatão dos Guararapes</t>
+  </si>
+  <si>
+    <t>Osasco</t>
+  </si>
+  <si>
+    <t>Uberlândia</t>
+  </si>
+  <si>
+    <t>Sorocaba</t>
+  </si>
+  <si>
+    <t>Contagem</t>
+  </si>
+  <si>
+    <t>Aracaju</t>
+  </si>
+  <si>
+    <t>Feira de Santana</t>
+  </si>
+  <si>
+    <t>Cuiabá</t>
+  </si>
+  <si>
+    <t>Joinville</t>
+  </si>
+  <si>
+    <t>Aparecida de Goiânia</t>
+  </si>
+  <si>
+    <t>Londrina</t>
+  </si>
+  <si>
+    <t>Juiz de Fora</t>
+  </si>
+  <si>
+    <t>Porto Velho</t>
+  </si>
+  <si>
+    <t>Ananindeua</t>
+  </si>
+  <si>
+    <t>Serra</t>
+  </si>
+  <si>
+    <t>Caxias do Sul</t>
+  </si>
+  <si>
+    <t>Niterói</t>
+  </si>
+  <si>
+    <t>Belford Roxo</t>
+  </si>
+  <si>
+    <t>Macapá</t>
+  </si>
+  <si>
+    <t>Campos dos Goytacazes</t>
+  </si>
+  <si>
+    <t>Florianópolis</t>
+  </si>
+  <si>
+    <t>Vila Velha</t>
+  </si>
+  <si>
+    <t>Mauá</t>
+  </si>
+  <si>
+    <t>São João de Meriti</t>
+  </si>
+  <si>
+    <t>São José do Rio Preto</t>
+  </si>
+  <si>
+    <t>Mogi das Cruzes</t>
+  </si>
+  <si>
+    <t>Betim</t>
+  </si>
+  <si>
+    <t>Santos</t>
+  </si>
+  <si>
+    <t>Maringá</t>
+  </si>
+  <si>
+    <t>Diadema</t>
+  </si>
+  <si>
+    <t>Jundiaí</t>
+  </si>
+  <si>
+    <t>Boa Vista</t>
+  </si>
+  <si>
+    <t>Montes Claros</t>
+  </si>
+  <si>
+    <t>Rio Branco</t>
+  </si>
+  <si>
+    <t>Campina Grande</t>
+  </si>
+  <si>
+    <t>Piracicaba</t>
+  </si>
+  <si>
+    <t>Carapicuíba</t>
+  </si>
+  <si>
+    <t>Olinda</t>
+  </si>
+  <si>
+    <t>Anápolis</t>
+  </si>
+  <si>
+    <t>Cariacica</t>
+  </si>
+  <si>
+    <t>Bauru</t>
+  </si>
+  <si>
+    <t>Itaquaquecetuba</t>
+  </si>
+  <si>
+    <t>São Vicente</t>
+  </si>
+  <si>
+    <t>Vitória</t>
+  </si>
+  <si>
+    <t>Caruaru</t>
+  </si>
+  <si>
+    <t>Caucaia</t>
+  </si>
+  <si>
+    <t>Blumenau</t>
+  </si>
+  <si>
+    <t>Franca</t>
+  </si>
+  <si>
+    <t>Ponta Grossa</t>
+  </si>
+  <si>
+    <t>Petrolina</t>
+  </si>
+  <si>
+    <t>Canoas</t>
+  </si>
+  <si>
+    <t>Pelotas</t>
+  </si>
+  <si>
+    <t>Vitória da Conquista</t>
+  </si>
+  <si>
+    <t>Ribeirão das Neves</t>
+  </si>
+  <si>
+    <t>Uberaba</t>
+  </si>
+  <si>
+    <t>Paulista</t>
+  </si>
+  <si>
+    <t>Cascavel</t>
+  </si>
+  <si>
+    <t>Praia Grande</t>
+  </si>
+  <si>
+    <t>São José dos Pinhais</t>
+  </si>
+  <si>
+    <t>Guarujá</t>
+  </si>
+  <si>
+    <t>Taubaté</t>
+  </si>
+  <si>
+    <t>Limeira</t>
+  </si>
+  <si>
+    <t>Petrópolis</t>
+  </si>
+  <si>
+    <t>Santarém</t>
+  </si>
+  <si>
+    <t>Palmas</t>
+  </si>
+  <si>
+    <t>Camaçari</t>
+  </si>
+  <si>
+    <t>Mossoró</t>
+  </si>
+  <si>
+    <t>Suzano</t>
+  </si>
+  <si>
+    <t>Taboão da Serra</t>
+  </si>
+  <si>
+    <t>Várzea Grande</t>
+  </si>
+  <si>
+    <t>Sumaré</t>
+  </si>
+  <si>
+    <t>Santa Maria</t>
+  </si>
+  <si>
+    <t>Gravataí</t>
+  </si>
+  <si>
+    <t>Marabá</t>
+  </si>
+  <si>
+    <t>Governador Valadares</t>
+  </si>
+  <si>
+    <t>Barueri</t>
+  </si>
+  <si>
+    <t>Embu das Artes</t>
+  </si>
+  <si>
+    <t>Juazeiro do Norte</t>
+  </si>
+  <si>
+    <t>Volta Redonda</t>
+  </si>
+  <si>
+    <t>Parnamirim</t>
+  </si>
+  <si>
+    <t>Ipatinga</t>
+  </si>
+  <si>
+    <t>Macaé</t>
+  </si>
+  <si>
+    <t>Imperatriz</t>
+  </si>
+  <si>
+    <t>Foz do Iguaçu</t>
+  </si>
+  <si>
+    <t>Viamão</t>
+  </si>
+  <si>
+    <t>Indaiatuba</t>
+  </si>
+  <si>
+    <t>São Carlos</t>
+  </si>
+  <si>
+    <t>Cotia</t>
+  </si>
+  <si>
+    <t>São José</t>
+  </si>
+  <si>
+    <t>Novo Hamburgo</t>
+  </si>
+  <si>
+    <t>Colombo</t>
+  </si>
+  <si>
+    <t>Magé</t>
+  </si>
+  <si>
+    <t>Itaboraí</t>
+  </si>
+  <si>
+    <t>Americana</t>
+  </si>
+  <si>
+    <t>Sete Lagoas</t>
+  </si>
+  <si>
+    <t>Rio Verde</t>
+  </si>
+  <si>
+    <t>Itapevi</t>
+  </si>
+  <si>
+    <t>Marília</t>
+  </si>
+  <si>
+    <t>Divinópolis</t>
+  </si>
+  <si>
+    <t>São Leopoldo</t>
+  </si>
+  <si>
+    <t>Araraquara</t>
+  </si>
+  <si>
+    <t>Rondonópolis</t>
+  </si>
+  <si>
+    <t>Jacareí</t>
+  </si>
+  <si>
+    <t>Hortolândia</t>
+  </si>
+  <si>
+    <t>Arapiraca</t>
+  </si>
+  <si>
+    <t>Cabo Frio</t>
+  </si>
+  <si>
+    <t>Presidente Prudente</t>
+  </si>
+  <si>
+    <t>Maracanaú</t>
+  </si>
+  <si>
+    <t>Dourados</t>
+  </si>
+  <si>
+    <t>Chapecó</t>
+  </si>
+  <si>
+    <t>Itajaí</t>
+  </si>
+  <si>
+    <t>Santa Luzia</t>
+  </si>
+  <si>
+    <t>Juazeiro</t>
+  </si>
+  <si>
+    <t>Águas Lindas de Goiás</t>
+  </si>
+  <si>
+    <t>Criciúma</t>
+  </si>
+  <si>
+    <t>Itabuna</t>
+  </si>
+  <si>
+    <t>Parauapebas</t>
+  </si>
+  <si>
+    <t>Rio Grande</t>
+  </si>
+  <si>
+    <t>Luziânia</t>
+  </si>
+  <si>
+    <t>Alvorada</t>
+  </si>
+  <si>
+    <t>Sobral</t>
+  </si>
+  <si>
+    <t>Cachoeiro de Itapemirim</t>
+  </si>
+  <si>
+    <t>Cabo de Santo Agostinho</t>
+  </si>
+  <si>
+    <t>Rio Claro</t>
+  </si>
+  <si>
+    <t>Angra dos Reis</t>
+  </si>
+  <si>
+    <t>Passo Fundo</t>
+  </si>
+  <si>
+    <t>Castanhal</t>
+  </si>
+  <si>
+    <t>Lauro de Freitas</t>
+  </si>
+  <si>
+    <t>Araçatuba</t>
+  </si>
+  <si>
+    <t>Ferraz de Vasconcelos</t>
+  </si>
+  <si>
+    <t>Santa Bárbara do Oeste</t>
+  </si>
+  <si>
+    <t>Nova Friburgo</t>
+  </si>
+  <si>
+    <t>Nossa Senhora do Socorro</t>
+  </si>
+  <si>
+    <t>Barra Mansa</t>
+  </si>
+  <si>
+    <t>Teresópolis</t>
+  </si>
+  <si>
+    <t>Araguaína</t>
+  </si>
+  <si>
+    <t>Guarapuava</t>
+  </si>
+  <si>
+    <t>Ibirité</t>
+  </si>
+  <si>
+    <t>Jaraguá do Sul</t>
+  </si>
+  <si>
+    <t>São José de Ribamar</t>
+  </si>
+  <si>
+    <t>Itapecerica da Serra</t>
+  </si>
+  <si>
+    <t>Francisco Morato</t>
+  </si>
+  <si>
+    <t>Linhares</t>
+  </si>
+  <si>
+    <t>Mesquita</t>
+  </si>
+  <si>
+    <t>Itu</t>
+  </si>
+  <si>
+    <t>Palhoça</t>
+  </si>
+  <si>
+    <t>Valparaíso de Goiás</t>
+  </si>
+  <si>
+    <t>Bragança Paulista</t>
+  </si>
+  <si>
+    <t>Timon</t>
+  </si>
+  <si>
+    <t>Pindamonhangaba</t>
+  </si>
+  <si>
+    <t>Poços de Caldas</t>
+  </si>
+  <si>
+    <t>Caxias</t>
+  </si>
+  <si>
+    <t>Maricá</t>
+  </si>
+  <si>
+    <t>Nilópolis</t>
+  </si>
+  <si>
+    <t>Teixeira de Freitas</t>
+  </si>
+  <si>
+    <t>São Caetano do Sul</t>
+  </si>
+  <si>
+    <t>Ilhéus</t>
+  </si>
+  <si>
+    <t>Abaetetuba</t>
+  </si>
+  <si>
+    <t>Camaragibe</t>
+  </si>
+  <si>
+    <t>Lages</t>
+  </si>
+  <si>
+    <t>Barreiras</t>
+  </si>
+  <si>
+    <t>Franco da Rocha</t>
+  </si>
+  <si>
+    <t>Paranaguá</t>
+  </si>
+  <si>
+    <t>Jequié</t>
+  </si>
+  <si>
+    <t>Rio das Ostras</t>
+  </si>
+  <si>
+    <t>Patos de Minas</t>
+  </si>
+  <si>
+    <t>Parnaíba</t>
+  </si>
+  <si>
+    <t>Mogi Guaçu</t>
+  </si>
+  <si>
+    <t>Pouso Alegre</t>
+  </si>
+  <si>
+    <t>Alagoinhas</t>
+  </si>
+  <si>
+    <t>Jaú</t>
+  </si>
+  <si>
+    <t>Queimados</t>
+  </si>
+  <si>
+    <t>RN</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>DF</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>GO</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>PB</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>TO</t>
+  </si>
+  <si>
+    <t>HILL, Napoleon. Mais Esperto Que O Diabo. 2021. - Editora: Citadel.</t>
+  </si>
+  <si>
+    <t>OBAMA, Barack. Uma Terra Prometida. 2021. - Editora: Companhia das Letras.</t>
+  </si>
+  <si>
+    <t>MANSON, Mark. A Sutil Arte De Ligar O Foda-Se. 2019. - Editora: Intrínseca.</t>
+  </si>
+  <si>
+    <t>PAUCAR, Pablo. Mentalidade. 2020. - Editora: Gente.</t>
+  </si>
+  <si>
+    <t>NIGRO, Thiago. Do Mil Ao Milhão. 2021. - Editora: HarperCollins.</t>
+  </si>
+  <si>
+    <t>MIRANDA, Felipe. Princípios Do Estrategista. 2021. - Editora: Intrínseca.</t>
+  </si>
+  <si>
+    <t>GASPAR, Malu. A Organização. 2019. - Editora: Companhia das Letras.</t>
+  </si>
+  <si>
+    <t>ESTES, Clarissa. Mulheres Que Correm Com Os Lobos. 2021. - Editora: Rocco.</t>
+  </si>
+  <si>
+    <t>ORWELL, George. A Revolução Dos Bichos. 2019. - Editora: Companhia das Letras.</t>
+  </si>
+  <si>
+    <t>VIEIRA, Paulo. O Poder Da Autorresponsabilidade. 2021. - Editora: Gente.</t>
+  </si>
+  <si>
+    <t>RIBEIRO, Djamila. Pequeno Manual Antirracista. 2021. - Editora: Companhia das Letras.</t>
+  </si>
+  <si>
+    <t>MEYER, Stephenie. Sol Da Meia-Noite. 2020. - Editora: Intrínseca.</t>
   </si>
 </sst>
 </file>
@@ -9985,7 +10699,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -10009,6 +10723,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -25629,7 +26344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1EC54E-C492-4397-9882-BC56FB77D447}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -25932,19 +26647,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71D899D-CD6F-4DFA-96B6-8BA0267A106F}">
-  <dimension ref="A1:E200"/>
+  <dimension ref="A1:F200"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="26.77734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.21875" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -25961,1796 +26678,3389 @@
         <v>403</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>3292</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2" s="5">
+        <v>12325232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>204</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>3293</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="5">
+        <v>6747815</v>
+      </c>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>205</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>3294</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3498</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="5">
+        <v>3055149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>206</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>3295</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3499</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="5">
+        <v>2886698</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>207</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>3296</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3500</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" s="5">
+        <v>2686612</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>208</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>3297</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" s="5">
+        <v>2521564</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>3298</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3501</v>
+      </c>
       <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" s="5">
+        <v>2219580</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>210</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>3299</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3502</v>
+      </c>
       <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" s="5">
+        <v>1948626</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>211</v>
       </c>
+      <c r="B10" s="1" t="s">
+        <v>3300</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3503</v>
+      </c>
       <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="5">
+        <v>1653461</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>212</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>3301</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3504</v>
+      </c>
       <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" s="5">
+        <v>1536097</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>213</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>3302</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3317</v>
+      </c>
       <c r="D12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" s="5">
+        <v>1499641</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>214</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3505</v>
+      </c>
       <c r="D13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13" s="5">
+        <v>1488252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>215</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>3304</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E14" s="5">
+        <v>1392121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>216</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>3305</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E15" s="5">
+        <v>1213792</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>217</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>3306</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3506</v>
+      </c>
       <c r="D16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="5">
+        <v>1108975</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>218</v>
       </c>
+      <c r="B17" s="1" t="s">
+        <v>3307</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="E17" s="5">
+        <v>1091737</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>219</v>
       </c>
+      <c r="B18" s="1" t="s">
+        <v>3308</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>3507</v>
+      </c>
       <c r="D18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="5">
+        <v>1025360</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>220</v>
       </c>
+      <c r="B19" s="1" t="s">
+        <v>3309</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="5">
+        <v>924624</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>221</v>
       </c>
+      <c r="B20" s="1" t="s">
+        <v>3310</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>3508</v>
+      </c>
       <c r="D20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="E20" s="5">
+        <v>906092</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>222</v>
       </c>
+      <c r="B21" s="1" t="s">
+        <v>3311</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>3494</v>
+      </c>
       <c r="D21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="E21" s="5">
+        <v>890480</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>223</v>
       </c>
+      <c r="B22" s="1" t="s">
+        <v>3312</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>3509</v>
+      </c>
       <c r="D22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="5">
+        <v>868075</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>224</v>
       </c>
+      <c r="B23" s="1" t="s">
+        <v>3313</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="5">
+        <v>844483</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>225</v>
       </c>
+      <c r="B24" s="1" t="s">
+        <v>3314</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E24" s="5">
+        <v>823302</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>226</v>
       </c>
+      <c r="B25" s="1" t="s">
+        <v>3318</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>3510</v>
+      </c>
       <c r="D25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="5">
+        <v>817511</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>227</v>
       </c>
+      <c r="B26" s="1" t="s">
+        <v>3319</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D26" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="E26" s="5">
+        <v>729737</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>228</v>
       </c>
+      <c r="B27" s="1" t="s">
+        <v>3320</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D27" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="5"/>
+      <c r="E27" s="5">
+        <v>721368</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>229</v>
       </c>
+      <c r="B28" s="1" t="s">
+        <v>3321</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="5"/>
+      <c r="E28" s="5">
+        <v>711825</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>230</v>
       </c>
+      <c r="B29" s="1" t="s">
+        <v>3322</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>3503</v>
+      </c>
       <c r="D29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="5"/>
+      <c r="E29" s="5">
+        <v>706867</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>231</v>
       </c>
+      <c r="B30" s="1" t="s">
+        <v>3323</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="E30" s="5">
+        <v>699944</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>232</v>
       </c>
+      <c r="B31" s="1" t="s">
+        <v>3324</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D31" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="E31" s="5">
+        <v>699097</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>233</v>
       </c>
+      <c r="B32" s="1" t="s">
+        <v>3325</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D32" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="E32" s="5">
+        <v>687357</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>234</v>
       </c>
+      <c r="B33" s="1" t="s">
+        <v>3326</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D33" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="E33" s="5">
+        <v>668949</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>235</v>
       </c>
+      <c r="B34" s="1" t="s">
+        <v>3327</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>3511</v>
+      </c>
       <c r="D34" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="E34" s="5">
+        <v>664908</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>236</v>
       </c>
+      <c r="B35" s="1" t="s">
+        <v>3328</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>3499</v>
+      </c>
       <c r="D35" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="5"/>
+      <c r="E35" s="5">
+        <v>619609</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>237</v>
       </c>
+      <c r="B36" s="1" t="s">
+        <v>3329</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>3512</v>
+      </c>
       <c r="D36" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="5"/>
+      <c r="E36" s="5">
+        <v>618124</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>238</v>
       </c>
+      <c r="B37" s="1" t="s">
+        <v>3330</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>3495</v>
+      </c>
       <c r="D37" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="5"/>
+      <c r="E37" s="5">
+        <v>597658</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>239</v>
       </c>
+      <c r="B38" s="1" t="s">
+        <v>3331</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>3504</v>
+      </c>
       <c r="D38" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="5"/>
+      <c r="E38" s="5">
+        <v>590146</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>240</v>
       </c>
+      <c r="B39" s="1" t="s">
+        <v>3332</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>3502</v>
+      </c>
       <c r="D39" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E39" s="5"/>
+      <c r="E39" s="5">
+        <v>575377</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>241</v>
       </c>
+      <c r="B40" s="1" t="s">
+        <v>3333</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D40" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="5"/>
+      <c r="E40" s="5">
+        <v>573285</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>242</v>
       </c>
+      <c r="B41" s="1" t="s">
+        <v>3334</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>3496</v>
+      </c>
       <c r="D41" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="5"/>
+      <c r="E41" s="5">
+        <v>539354</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>243</v>
       </c>
+      <c r="B42" s="1" t="s">
+        <v>3335</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>3317</v>
+      </c>
       <c r="D42" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E42" s="5"/>
+      <c r="E42" s="5">
+        <v>535547</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>244</v>
       </c>
+      <c r="B43" s="1" t="s">
+        <v>3336</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>3513</v>
+      </c>
       <c r="D43" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E43" s="5"/>
+      <c r="E43" s="5">
+        <v>527240</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>245</v>
       </c>
+      <c r="B44" s="1" t="s">
+        <v>3337</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>3505</v>
+      </c>
       <c r="D44" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="5"/>
+      <c r="E44" s="5">
+        <v>517451</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="B45" s="1" t="s">
+        <v>3338</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D45" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E45" s="5"/>
+      <c r="E45" s="5">
+        <v>515317</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>247</v>
       </c>
+      <c r="B46" s="1" t="s">
+        <v>3339</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D46" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E46" s="5"/>
+      <c r="E46" s="5">
+        <v>513118</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>248</v>
       </c>
+      <c r="B47" s="1" t="s">
+        <v>3340</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>3514</v>
+      </c>
       <c r="D47" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E47" s="5"/>
+      <c r="E47" s="5">
+        <v>512902</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>249</v>
       </c>
+      <c r="B48" s="1" t="s">
+        <v>3341</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D48" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E48" s="5"/>
+      <c r="E48" s="5">
+        <v>511168</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>250</v>
       </c>
+      <c r="B49" s="1" t="s">
+        <v>3342</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>3495</v>
+      </c>
       <c r="D49" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E49" s="5"/>
+      <c r="E49" s="5">
+        <v>508826</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>251</v>
       </c>
+      <c r="B50" s="1" t="s">
+        <v>3343</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>3513</v>
+      </c>
       <c r="D50" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E50" s="5"/>
+      <c r="E50" s="5">
+        <v>501325</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>252</v>
       </c>
+      <c r="B51" s="1" t="s">
+        <v>3344</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D51" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E51" s="5"/>
+      <c r="E51" s="5">
+        <v>477552</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>253</v>
       </c>
+      <c r="B52" s="1" t="s">
+        <v>3345</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D52" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E52" s="5"/>
+      <c r="E52" s="5">
+        <v>472906</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>254</v>
       </c>
+      <c r="B53" s="1" t="s">
+        <v>3346</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D53" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E53" s="5"/>
+      <c r="E53" s="5">
+        <v>464983</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>255</v>
       </c>
+      <c r="B54" s="1" t="s">
+        <v>3347</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D54" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E54" s="5"/>
+      <c r="E54" s="5">
+        <v>450785</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>256</v>
       </c>
+      <c r="B55" s="1" t="s">
+        <v>3348</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D55" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="5"/>
+      <c r="E55" s="5">
+        <v>444784</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>257</v>
       </c>
+      <c r="B56" s="1" t="s">
+        <v>3349</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D56" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E56" s="5"/>
+      <c r="E56" s="5">
+        <v>433656</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>258</v>
       </c>
+      <c r="B57" s="1" t="s">
+        <v>3350</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>3502</v>
+      </c>
       <c r="D57" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E57" s="5"/>
+      <c r="E57" s="5">
+        <v>430157</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>259</v>
       </c>
+      <c r="B58" s="1" t="s">
+        <v>3351</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D58" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E58" s="5"/>
+      <c r="E58" s="5">
+        <v>426757</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>260</v>
       </c>
+      <c r="B59" s="1" t="s">
+        <v>3352</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D59" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E59" s="5"/>
+      <c r="E59" s="5">
+        <v>423006</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>261</v>
       </c>
+      <c r="B60" s="1" t="s">
+        <v>3353</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>3515</v>
+      </c>
       <c r="D60" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E60" s="5"/>
+      <c r="E60" s="5">
+        <v>419652</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>262</v>
       </c>
+      <c r="B61" s="1" t="s">
+        <v>3354</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D61" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E61" s="5"/>
+      <c r="E61" s="5">
+        <v>413487</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>263</v>
       </c>
+      <c r="B62" s="1" t="s">
+        <v>3355</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>3516</v>
+      </c>
       <c r="D62" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E62" s="5"/>
+      <c r="E62" s="5">
+        <v>413418</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>264</v>
       </c>
+      <c r="B63" s="1" t="s">
+        <v>3356</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>3510</v>
+      </c>
       <c r="D63" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E63" s="5"/>
+      <c r="E63" s="5">
+        <v>411807</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>265</v>
       </c>
+      <c r="B64" s="1" t="s">
+        <v>3357</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D64" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E64" s="5"/>
+      <c r="E64" s="5">
+        <v>407252</v>
+      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>266</v>
       </c>
+      <c r="B65" s="1" t="s">
+        <v>3358</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D65" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E65" s="5"/>
+      <c r="E65" s="5">
+        <v>403183</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>267</v>
       </c>
+      <c r="B66" s="1" t="s">
+        <v>3359</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>3503</v>
+      </c>
       <c r="D66" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E66" s="5"/>
+      <c r="E66" s="5">
+        <v>393115</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>268</v>
       </c>
+      <c r="B67" s="1" t="s">
+        <v>3360</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>3504</v>
+      </c>
       <c r="D67" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E67" s="5"/>
+      <c r="E67" s="5">
+        <v>391772</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>269</v>
       </c>
+      <c r="B68" s="1" t="s">
+        <v>3361</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>3513</v>
+      </c>
       <c r="D68" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E68" s="5"/>
+      <c r="E68" s="5">
+        <v>383917</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>270</v>
       </c>
+      <c r="B69" s="1" t="s">
+        <v>3362</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D69" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E69" s="5"/>
+      <c r="E69" s="5">
+        <v>379297</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>271</v>
       </c>
+      <c r="B70" s="1" t="s">
+        <v>3363</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D70" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E70" s="5"/>
+      <c r="E70" s="5">
+        <v>375011</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>272</v>
       </c>
+      <c r="B71" s="1" t="s">
+        <v>3364</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D71" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E71" s="5"/>
+      <c r="E71" s="5">
+        <v>368355</v>
+      </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>273</v>
       </c>
+      <c r="B72" s="1" t="s">
+        <v>3365</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>3513</v>
+      </c>
       <c r="D72" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E72" s="5"/>
+      <c r="E72" s="5">
+        <v>365855</v>
+      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>274</v>
       </c>
+      <c r="B73" s="1" t="s">
+        <v>3366</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>3503</v>
+      </c>
       <c r="D73" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E73" s="5"/>
+      <c r="E73" s="5">
+        <v>365278</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>275</v>
       </c>
+      <c r="B74" s="1" t="s">
+        <v>3367</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>3500</v>
+      </c>
       <c r="D74" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E74" s="5"/>
+      <c r="E74" s="5">
+        <v>365212</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>276</v>
       </c>
+      <c r="B75" s="1" t="s">
+        <v>3368</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>3495</v>
+      </c>
       <c r="D75" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E75" s="5"/>
+      <c r="E75" s="5">
+        <v>361855</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>277</v>
       </c>
+      <c r="B76" s="1" t="s">
+        <v>3369</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D76" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E76" s="5"/>
+      <c r="E76" s="5">
+        <v>355901</v>
+      </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>278</v>
       </c>
+      <c r="B77" s="1" t="s">
+        <v>3370</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>3502</v>
+      </c>
       <c r="D77" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E77" s="5"/>
+      <c r="E77" s="5">
+        <v>355336</v>
+      </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>279</v>
       </c>
+      <c r="B78" s="1" t="s">
+        <v>3371</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>3503</v>
+      </c>
       <c r="D78" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E78" s="5"/>
+      <c r="E78" s="5">
+        <v>354317</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>280</v>
       </c>
+      <c r="B79" s="1" t="s">
+        <v>3372</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>3505</v>
+      </c>
       <c r="D79" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E79" s="5"/>
+      <c r="E79" s="5">
+        <v>348208</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>281</v>
       </c>
+      <c r="B80" s="1" t="s">
+        <v>3373</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>3505</v>
+      </c>
       <c r="D80" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E80" s="5"/>
+      <c r="E80" s="5">
+        <v>343132</v>
+      </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>282</v>
       </c>
+      <c r="B81" s="1" t="s">
+        <v>3374</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>3499</v>
+      </c>
       <c r="D81" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E81" s="5"/>
+      <c r="E81" s="5">
+        <v>341128</v>
+      </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>283</v>
       </c>
+      <c r="B82" s="1" t="s">
+        <v>3375</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D82" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E82" s="5"/>
+      <c r="E82" s="5">
+        <v>338197</v>
+      </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>284</v>
       </c>
+      <c r="B83" s="1" t="s">
+        <v>3376</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D83" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E83" s="5"/>
+      <c r="E83" s="5">
+        <v>337092</v>
+      </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>285</v>
       </c>
+      <c r="B84" s="1" t="s">
+        <v>3377</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>3503</v>
+      </c>
       <c r="D84" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E84" s="5"/>
+      <c r="E84" s="5">
+        <v>334376</v>
+      </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>286</v>
       </c>
+      <c r="B85" s="1" t="s">
+        <v>3378</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>3502</v>
+      </c>
       <c r="D85" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E85" s="5"/>
+      <c r="E85" s="5">
+        <v>332333</v>
+      </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>287</v>
       </c>
+      <c r="B86" s="1" t="s">
+        <v>3379</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D86" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E86" s="5"/>
+      <c r="E86" s="5">
+        <v>330845</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>288</v>
       </c>
+      <c r="B87" s="1" t="s">
+        <v>3380</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>3502</v>
+      </c>
       <c r="D87" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E87" s="5"/>
+      <c r="E87" s="5">
+        <v>329058</v>
+      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>289</v>
       </c>
+      <c r="B88" s="1" t="s">
+        <v>3381</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D88" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E88" s="5"/>
+      <c r="E88" s="5">
+        <v>322750</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>290</v>
       </c>
+      <c r="B89" s="1" t="s">
+        <v>3382</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D89" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E89" s="5"/>
+      <c r="E89" s="5">
+        <v>317915</v>
+      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>291</v>
       </c>
+      <c r="B90" s="1" t="s">
+        <v>3383</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D90" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E90" s="5"/>
+      <c r="E90" s="5">
+        <v>308482</v>
+      </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>292</v>
       </c>
+      <c r="B91" s="1" t="s">
+        <v>3384</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D91" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E91" s="5"/>
+      <c r="E91" s="5">
+        <v>306678</v>
+      </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>293</v>
       </c>
+      <c r="B92" s="1" t="s">
+        <v>3385</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>3317</v>
+      </c>
       <c r="D92" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E92" s="5"/>
+      <c r="E92" s="5">
+        <v>306480</v>
+      </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>294</v>
       </c>
+      <c r="B93" s="1" t="s">
+        <v>3386</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>3517</v>
+      </c>
       <c r="D93" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E93" s="5"/>
+      <c r="E93" s="5">
+        <v>306296</v>
+      </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>295</v>
       </c>
+      <c r="B94" s="1" t="s">
+        <v>3387</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>3499</v>
+      </c>
       <c r="D94" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E94" s="5"/>
+      <c r="E94" s="5">
+        <v>304302</v>
+      </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>296</v>
       </c>
+      <c r="B95" s="1" t="s">
+        <v>3388</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>3494</v>
+      </c>
       <c r="D95" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E95" s="5"/>
+      <c r="E95" s="5">
+        <v>300618</v>
+      </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>297</v>
       </c>
+      <c r="B96" s="1" t="s">
+        <v>3389</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D96" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E96" s="5"/>
+      <c r="E96" s="5">
+        <v>300559</v>
+      </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>298</v>
       </c>
+      <c r="B97" s="1" t="s">
+        <v>3390</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D97" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E97" s="5"/>
+      <c r="E97" s="5">
+        <v>293652</v>
+      </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>299</v>
       </c>
+      <c r="B98" s="1" t="s">
+        <v>3391</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>3512</v>
+      </c>
       <c r="D98" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E98" s="5"/>
+      <c r="E98" s="5">
+        <v>287526</v>
+      </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>300</v>
       </c>
+      <c r="B99" s="1" t="s">
+        <v>3392</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D99" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E99" s="5"/>
+      <c r="E99" s="5">
+        <v>286211</v>
+      </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>301</v>
       </c>
+      <c r="B100" s="1" t="s">
+        <v>3393</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>3505</v>
+      </c>
       <c r="D100" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E100" s="5"/>
+      <c r="E100" s="5">
+        <v>283677</v>
+      </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>302</v>
       </c>
+      <c r="B101" s="1" t="s">
+        <v>3394</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>3505</v>
+      </c>
       <c r="D101" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E101" s="5"/>
+      <c r="E101" s="5">
+        <v>283620</v>
+      </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>303</v>
       </c>
+      <c r="B102" s="1" t="s">
+        <v>3395</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>3317</v>
+      </c>
       <c r="D102" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E102" s="5"/>
+      <c r="E102" s="5">
+        <v>283542</v>
+      </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>304</v>
       </c>
+      <c r="B103" s="1" t="s">
+        <v>3396</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D103" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E103" s="5"/>
+      <c r="E103" s="5">
+        <v>281046</v>
+      </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>305</v>
       </c>
+      <c r="B104" s="1" t="s">
+        <v>3397</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D104" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E104" s="5"/>
+      <c r="E104" s="5">
+        <v>276982</v>
+      </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>306</v>
       </c>
+      <c r="B105" s="1" t="s">
+        <v>3398</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D105" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E105" s="5"/>
+      <c r="E105" s="5">
+        <v>276535</v>
+      </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>307</v>
       </c>
+      <c r="B106" s="1" t="s">
+        <v>3399</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>3500</v>
+      </c>
       <c r="D106" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E106" s="5"/>
+      <c r="E106" s="5">
+        <v>276264</v>
+      </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>308</v>
       </c>
+      <c r="B107" s="1" t="s">
+        <v>3400</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D107" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E107" s="5"/>
+      <c r="E107" s="5">
+        <v>273988</v>
+      </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>309</v>
       </c>
+      <c r="B108" s="1" t="s">
+        <v>3401</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>3494</v>
+      </c>
       <c r="D108" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E108" s="5"/>
+      <c r="E108" s="5">
+        <v>267036</v>
+      </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>310</v>
       </c>
+      <c r="B109" s="1" t="s">
+        <v>3402</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D109" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E109" s="5"/>
+      <c r="E109" s="5">
+        <v>265409</v>
+      </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="B110" s="1" t="s">
+        <v>3403</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D110" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E110" s="5"/>
+      <c r="E110" s="5">
+        <v>261501</v>
+      </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>312</v>
       </c>
+      <c r="B111" s="1" t="s">
+        <v>3404</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>3506</v>
+      </c>
       <c r="D111" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E111" s="5"/>
+      <c r="E111" s="5">
+        <v>259337</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>313</v>
       </c>
+      <c r="B112" s="1" t="s">
+        <v>3405</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>3502</v>
+      </c>
       <c r="D112" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E112" s="5"/>
+      <c r="E112" s="5">
+        <v>258248</v>
+      </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>314</v>
       </c>
+      <c r="B113" s="1" t="s">
+        <v>3406</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>3505</v>
+      </c>
       <c r="D113" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E113" s="5"/>
+      <c r="E113" s="5">
+        <v>256302</v>
+      </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>315</v>
       </c>
+      <c r="B114" s="1" t="s">
+        <v>3407</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D114" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E114" s="5"/>
+      <c r="E114" s="5">
+        <v>256223</v>
+      </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>316</v>
       </c>
+      <c r="B115" s="1" t="s">
+        <v>3408</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D115" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E115" s="5"/>
+      <c r="E115" s="5">
+        <v>254484</v>
+      </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>317</v>
       </c>
+      <c r="B116" s="1" t="s">
+        <v>3409</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D116" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E116" s="5"/>
+      <c r="E116" s="5">
+        <v>253608</v>
+      </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>318</v>
       </c>
+      <c r="B117" s="1" t="s">
+        <v>3410</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>3495</v>
+      </c>
       <c r="D117" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E117" s="5"/>
+      <c r="E117" s="5">
+        <v>250181</v>
+      </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>319</v>
       </c>
+      <c r="B118" s="1" t="s">
+        <v>3411</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>3505</v>
+      </c>
       <c r="D118" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E118" s="5"/>
+      <c r="E118" s="5">
+        <v>247032</v>
+      </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>320</v>
       </c>
+      <c r="B119" s="1" t="s">
+        <v>3412</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>3502</v>
+      </c>
       <c r="D119" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E119" s="5"/>
+      <c r="E119" s="5">
+        <v>246540</v>
+      </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>321</v>
       </c>
+      <c r="B120" s="1" t="s">
+        <v>3413</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D120" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E120" s="5"/>
+      <c r="E120" s="5">
+        <v>246433</v>
+      </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>322</v>
       </c>
+      <c r="B121" s="1" t="s">
+        <v>3414</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D121" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E121" s="5"/>
+      <c r="E121" s="5">
+        <v>242543</v>
+      </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>323</v>
       </c>
+      <c r="B122" s="1" t="s">
+        <v>3415</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D122" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E122" s="5"/>
+      <c r="E122" s="5">
+        <v>242018</v>
+      </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>324</v>
       </c>
+      <c r="B123" s="1" t="s">
+        <v>3416</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D123" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E123" s="5"/>
+      <c r="E123" s="5">
+        <v>241835</v>
+      </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>325</v>
       </c>
+      <c r="B124" s="1" t="s">
+        <v>3417</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>3504</v>
+      </c>
       <c r="D124" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E124" s="5"/>
+      <c r="E124" s="5">
+        <v>241518</v>
+      </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>326</v>
       </c>
+      <c r="B125" s="1" t="s">
+        <v>3418</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D125" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E125" s="5"/>
+      <c r="E125" s="5">
+        <v>240961</v>
+      </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>327</v>
       </c>
+      <c r="B126" s="1" t="s">
+        <v>3419</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D126" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E126" s="5"/>
+      <c r="E126" s="5">
+        <v>240590</v>
+      </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="B127" s="1" t="s">
+        <v>3420</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D127" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E127" s="5"/>
+      <c r="E127" s="5">
+        <v>240408</v>
+      </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>329</v>
       </c>
+      <c r="B128" s="1" t="s">
+        <v>3421</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>3505</v>
+      </c>
       <c r="D128" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E128" s="5"/>
+      <c r="E128" s="5">
+        <v>238648</v>
+      </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>330</v>
       </c>
+      <c r="B129" s="1" t="s">
+        <v>3422</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D129" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E129" s="5"/>
+      <c r="E129" s="5">
+        <v>238339</v>
+      </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>331</v>
       </c>
+      <c r="B130" s="1" t="s">
+        <v>3423</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>3512</v>
+      </c>
       <c r="D130" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E130" s="5"/>
+      <c r="E130" s="5">
+        <v>236042</v>
+      </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>332</v>
       </c>
+      <c r="B131" s="1" t="s">
+        <v>3424</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D131" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E131" s="5"/>
+      <c r="E131" s="5">
+        <v>235416</v>
+      </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>333</v>
       </c>
+      <c r="B132" s="1" t="s">
+        <v>3425</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D132" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E132" s="5"/>
+      <c r="E132" s="5">
+        <v>234259</v>
+      </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>334</v>
       </c>
+      <c r="B133" s="1" t="s">
+        <v>3426</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>3507</v>
+      </c>
       <c r="D133" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E133" s="5"/>
+      <c r="E133" s="5">
+        <v>233047</v>
+      </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>335</v>
       </c>
+      <c r="B134" s="1" t="s">
+        <v>3427</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D134" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E134" s="5"/>
+      <c r="E134" s="5">
+        <v>230378</v>
+      </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>336</v>
       </c>
+      <c r="B135" s="1" t="s">
+        <v>3428</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D135" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E135" s="5"/>
+      <c r="E135" s="5">
+        <v>230371</v>
+      </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>337</v>
       </c>
+      <c r="B136" s="1" t="s">
+        <v>3429</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>3500</v>
+      </c>
       <c r="D136" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E136" s="5"/>
+      <c r="E136" s="5">
+        <v>229458</v>
+      </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>338</v>
       </c>
+      <c r="B137" s="1" t="s">
+        <v>3430</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>3508</v>
+      </c>
       <c r="D137" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E137" s="5"/>
+      <c r="E137" s="5">
+        <v>225495</v>
+      </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>339</v>
       </c>
+      <c r="B138" s="1" t="s">
+        <v>3431</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>3495</v>
+      </c>
       <c r="D138" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E138" s="5"/>
+      <c r="E138" s="5">
+        <v>224013</v>
+      </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>340</v>
       </c>
+      <c r="B139" s="1" t="s">
+        <v>3432</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>3495</v>
+      </c>
       <c r="D139" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E139" s="5"/>
+      <c r="E139" s="5">
+        <v>223112</v>
+      </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>341</v>
       </c>
+      <c r="B140" s="1" t="s">
+        <v>3433</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D140" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E140" s="5"/>
+      <c r="E140" s="5">
+        <v>220444</v>
+      </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>342</v>
       </c>
+      <c r="B141" s="1" t="s">
+        <v>3434</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>3499</v>
+      </c>
       <c r="D141" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E141" s="5"/>
+      <c r="E141" s="5">
+        <v>218162</v>
+      </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>343</v>
       </c>
+      <c r="B142" s="1" t="s">
+        <v>3435</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>3504</v>
+      </c>
       <c r="D142" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E142" s="5"/>
+      <c r="E142" s="5">
+        <v>217698</v>
+      </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>344</v>
       </c>
+      <c r="B143" s="1" t="s">
+        <v>3436</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>3495</v>
+      </c>
       <c r="D143" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E143" s="5"/>
+      <c r="E143" s="5">
+        <v>217311</v>
+      </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>345</v>
       </c>
+      <c r="B144" s="1" t="s">
+        <v>3437</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>3499</v>
+      </c>
       <c r="D144" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="E144" s="5"/>
+      <c r="E144" s="5">
+        <v>213685</v>
+      </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>346</v>
       </c>
+      <c r="B145" s="1" t="s">
+        <v>3438</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>3317</v>
+      </c>
       <c r="D145" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E145" s="5"/>
+      <c r="E145" s="5">
+        <v>213576</v>
+      </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>347</v>
       </c>
+      <c r="B146" s="1" t="s">
+        <v>3439</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>3505</v>
+      </c>
       <c r="D146" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E146" s="5"/>
+      <c r="E146" s="5">
+        <v>211965</v>
+      </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>348</v>
       </c>
+      <c r="B147" s="1" t="s">
+        <v>3440</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>3504</v>
+      </c>
       <c r="D147" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E147" s="5"/>
+      <c r="E147" s="5">
+        <v>211508</v>
+      </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>349</v>
       </c>
+      <c r="B148" s="1" t="s">
+        <v>3441</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>3505</v>
+      </c>
       <c r="D148" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E148" s="5"/>
+      <c r="E148" s="5">
+        <v>211352</v>
+      </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>350</v>
       </c>
+      <c r="B149" s="1" t="s">
+        <v>3442</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>3500</v>
+      </c>
       <c r="D149" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E149" s="5"/>
+      <c r="E149" s="5">
+        <v>210711</v>
+      </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>351</v>
       </c>
+      <c r="B150" s="1" t="s">
+        <v>3443</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>3513</v>
+      </c>
       <c r="D150" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E150" s="5"/>
+      <c r="E150" s="5">
+        <v>210589</v>
+      </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>352</v>
       </c>
+      <c r="B151" s="1" t="s">
+        <v>3444</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>3503</v>
+      </c>
       <c r="D151" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E151" s="5"/>
+      <c r="E151" s="5">
+        <v>208944</v>
+      </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>353</v>
       </c>
+      <c r="B152" s="1" t="s">
+        <v>3445</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D152" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E152" s="5"/>
+      <c r="E152" s="5">
+        <v>208008</v>
+      </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>354</v>
       </c>
+      <c r="B153" s="1" t="s">
+        <v>3446</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D153" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E153" s="5"/>
+      <c r="E153" s="5">
+        <v>207044</v>
+      </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>355</v>
       </c>
+      <c r="B154" s="1" t="s">
+        <v>3447</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>3505</v>
+      </c>
       <c r="D154" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E154" s="5"/>
+      <c r="E154" s="5">
+        <v>204722</v>
+      </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>356</v>
       </c>
+      <c r="B155" s="1" t="s">
+        <v>3448</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>3317</v>
+      </c>
       <c r="D155" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="E155" s="5"/>
+      <c r="E155" s="5">
+        <v>203251</v>
+      </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>357</v>
       </c>
+      <c r="B156" s="1" t="s">
+        <v>3449</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>3499</v>
+      </c>
       <c r="D156" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E156" s="5"/>
+      <c r="E156" s="5">
+        <v>201635</v>
+      </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>358</v>
       </c>
+      <c r="B157" s="1" t="s">
+        <v>3450</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D157" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E157" s="5"/>
+      <c r="E157" s="5">
+        <v>198129</v>
+      </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>359</v>
       </c>
+      <c r="B158" s="1" t="s">
+        <v>3451</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D158" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E158" s="5"/>
+      <c r="E158" s="5">
+        <v>196500</v>
+      </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>360</v>
       </c>
+      <c r="B159" s="1" t="s">
+        <v>3452</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D159" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="E159" s="5"/>
+      <c r="E159" s="5">
+        <v>194390</v>
+      </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>361</v>
       </c>
+      <c r="B160" s="1" t="s">
+        <v>3453</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D160" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E160" s="5"/>
+      <c r="E160" s="5">
+        <v>191158</v>
+      </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>362</v>
       </c>
+      <c r="B161" s="1" t="s">
+        <v>3454</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>3511</v>
+      </c>
       <c r="D161" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E161" s="5"/>
+      <c r="E161" s="5">
+        <v>185706</v>
+      </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>363</v>
       </c>
+      <c r="B162" s="1" t="s">
+        <v>3455</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D162" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E162" s="5"/>
+      <c r="E162" s="5">
+        <v>184833</v>
+      </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>364</v>
       </c>
+      <c r="B163" s="1" t="s">
+        <v>3456</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D163" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="E163" s="5"/>
+      <c r="E163" s="5">
+        <v>184240</v>
+      </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>365</v>
       </c>
+      <c r="B164" s="1" t="s">
+        <v>3457</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>3517</v>
+      </c>
       <c r="D164" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E164" s="5"/>
+      <c r="E164" s="5">
+        <v>183381</v>
+      </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>366</v>
       </c>
+      <c r="B165" s="1" t="s">
+        <v>3458</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>3502</v>
+      </c>
       <c r="D165" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="E165" s="5"/>
+      <c r="E165" s="5">
+        <v>182644</v>
+      </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>367</v>
       </c>
+      <c r="B166" s="1" t="s">
+        <v>3459</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D166" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="E166" s="5"/>
+      <c r="E166" s="5">
+        <v>182153</v>
+      </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>368</v>
       </c>
+      <c r="B167" s="1" t="s">
+        <v>3460</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>3495</v>
+      </c>
       <c r="D167" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="E167" s="5"/>
+      <c r="E167" s="5">
+        <v>181173</v>
+      </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>369</v>
       </c>
+      <c r="B168" s="1" t="s">
+        <v>3461</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>3506</v>
+      </c>
       <c r="D168" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="E168" s="5"/>
+      <c r="E168" s="5">
+        <v>179028</v>
+      </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>370</v>
       </c>
+      <c r="B169" s="1" t="s">
+        <v>3462</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D169" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E169" s="5"/>
+      <c r="E169" s="5">
+        <v>177662</v>
+      </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>371</v>
       </c>
+      <c r="B170" s="1" t="s">
+        <v>3463</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D170" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="E170" s="5"/>
+      <c r="E170" s="5">
+        <v>177633</v>
+      </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>372</v>
       </c>
+      <c r="B171" s="1" t="s">
+        <v>3464</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>3513</v>
+      </c>
       <c r="D171" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E171" s="5"/>
+      <c r="E171" s="5">
+        <v>176688</v>
+      </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>373</v>
       </c>
+      <c r="B172" s="1" t="s">
+        <v>3465</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D172" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E172" s="5"/>
+      <c r="E172" s="5">
+        <v>176569</v>
+      </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>374</v>
       </c>
+      <c r="B173" s="1" t="s">
+        <v>3466</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D173" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="E173" s="5"/>
+      <c r="E173" s="5">
+        <v>175568</v>
+      </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>375</v>
       </c>
+      <c r="B174" s="1" t="s">
+        <v>3467</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>3495</v>
+      </c>
       <c r="D174" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E174" s="5"/>
+      <c r="E174" s="5">
+        <v>175272</v>
+      </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>376</v>
       </c>
+      <c r="B175" s="1" t="s">
+        <v>3468</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>3504</v>
+      </c>
       <c r="D175" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="E175" s="5"/>
+      <c r="E175" s="5">
+        <v>172135</v>
+      </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>377</v>
       </c>
+      <c r="B176" s="1" t="s">
+        <v>3469</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D176" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E176" s="5"/>
+      <c r="E176" s="5">
+        <v>170533</v>
+      </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>378</v>
       </c>
+      <c r="B177" s="1" t="s">
+        <v>3470</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>3506</v>
+      </c>
       <c r="D177" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E177" s="5"/>
+      <c r="E177" s="5">
+        <v>170222</v>
+      </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>379</v>
       </c>
+      <c r="B178" s="1" t="s">
+        <v>3471</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D178" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="E178" s="5"/>
+      <c r="E178" s="5">
+        <v>170132</v>
+      </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>380</v>
       </c>
+      <c r="B179" s="1" t="s">
+        <v>3472</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D179" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E179" s="5"/>
+      <c r="E179" s="5">
+        <v>168641</v>
+      </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>381</v>
       </c>
+      <c r="B180" s="1" t="s">
+        <v>3473</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>3506</v>
+      </c>
       <c r="D180" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="E180" s="5"/>
+      <c r="E180" s="5">
+        <v>165525</v>
+      </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>382</v>
       </c>
+      <c r="B181" s="1" t="s">
+        <v>3474</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D181" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="E181" s="5"/>
+      <c r="E181" s="5">
+        <v>164504</v>
+      </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>383</v>
       </c>
+      <c r="B182" s="1" t="s">
+        <v>3475</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D182" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E182" s="5"/>
+      <c r="E182" s="5">
+        <v>162693</v>
+      </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>384</v>
       </c>
+      <c r="B183" s="1" t="s">
+        <v>3476</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>3499</v>
+      </c>
       <c r="D183" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="E183" s="5"/>
+      <c r="E183" s="5">
+        <v>162438</v>
+      </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>385</v>
       </c>
+      <c r="B184" s="1" t="s">
+        <v>3477</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D184" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="E184" s="5"/>
+      <c r="E184" s="5">
+        <v>161957</v>
+      </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>386</v>
       </c>
+      <c r="B185" s="1" t="s">
+        <v>3478</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>3499</v>
+      </c>
       <c r="D185" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="E185" s="5"/>
+      <c r="E185" s="5">
+        <v>159923</v>
+      </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>387</v>
       </c>
+      <c r="B186" s="1" t="s">
+        <v>3479</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>3317</v>
+      </c>
       <c r="D186" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="E186" s="5"/>
+      <c r="E186" s="5">
+        <v>159080</v>
+      </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>388</v>
       </c>
+      <c r="B187" s="1" t="s">
+        <v>3480</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>3503</v>
+      </c>
       <c r="D187" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="E187" s="5"/>
+      <c r="E187" s="5">
+        <v>158899</v>
+      </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>389</v>
       </c>
+      <c r="B188" s="1" t="s">
+        <v>3481</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>3495</v>
+      </c>
       <c r="D188" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="E188" s="5"/>
+      <c r="E188" s="5">
+        <v>157349</v>
+      </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>390</v>
       </c>
+      <c r="B189" s="1" t="s">
+        <v>3482</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>3499</v>
+      </c>
       <c r="D189" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="E189" s="5"/>
+      <c r="E189" s="5">
+        <v>156975</v>
+      </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>391</v>
       </c>
+      <c r="B190" s="1" t="s">
+        <v>3483</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D190" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="E190" s="5"/>
+      <c r="E190" s="5">
+        <v>156492</v>
+      </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>392</v>
       </c>
+      <c r="B191" s="1" t="s">
+        <v>3484</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>3502</v>
+      </c>
       <c r="D191" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="E191" s="5"/>
+      <c r="E191" s="5">
+        <v>156174</v>
+      </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>393</v>
       </c>
+      <c r="B192" s="1" t="s">
+        <v>3485</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>3499</v>
+      </c>
       <c r="D192" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="E192" s="5"/>
+      <c r="E192" s="5">
+        <v>156126</v>
+      </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>394</v>
       </c>
+      <c r="B193" s="1" t="s">
+        <v>3486</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D193" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="E193" s="5"/>
+      <c r="E193" s="5">
+        <v>155193</v>
+      </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>395</v>
       </c>
+      <c r="B194" s="1" t="s">
+        <v>3487</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D194" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E194" s="5"/>
+      <c r="E194" s="5">
+        <v>153585</v>
+      </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>396</v>
       </c>
+      <c r="B195" s="1" t="s">
+        <v>3488</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>3509</v>
+      </c>
       <c r="D195" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="E195" s="5"/>
+      <c r="E195" s="5">
+        <v>153482</v>
+      </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>397</v>
       </c>
+      <c r="B196" s="1" t="s">
+        <v>3489</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D196" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E196" s="5"/>
+      <c r="E196" s="5">
+        <v>153033</v>
+      </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>398</v>
       </c>
+      <c r="B197" s="1" t="s">
+        <v>3490</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>3497</v>
+      </c>
       <c r="D197" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="E197" s="5"/>
+      <c r="E197" s="5">
+        <v>152549</v>
+      </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>399</v>
       </c>
+      <c r="B198" s="1" t="s">
+        <v>3491</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>3499</v>
+      </c>
       <c r="D198" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E198" s="5"/>
+      <c r="E198" s="5">
+        <v>152327</v>
+      </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>400</v>
       </c>
+      <c r="B199" s="1" t="s">
+        <v>3492</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>3315</v>
+      </c>
       <c r="D199" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="E199" s="5"/>
+      <c r="E199" s="5">
+        <v>151881</v>
+      </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>401</v>
       </c>
+      <c r="B200" s="1" t="s">
+        <v>3493</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>3316</v>
+      </c>
       <c r="D200" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E200" s="5"/>
+      <c r="E200" s="5">
+        <v>151335</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -27761,7 +30071,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42EE139-623A-4D62-899E-10CF8EBDA1E8}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -27819,7 +30131,9 @@
       <c r="D3" s="1">
         <v>2021</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>3518</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -27834,7 +30148,9 @@
       <c r="D4" s="1">
         <v>2021</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>3519</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -27849,7 +30165,9 @@
       <c r="D5" s="1">
         <v>2019</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>3520</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -27864,7 +30182,9 @@
       <c r="D6" s="1">
         <v>2020</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>3521</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -27879,7 +30199,9 @@
       <c r="D7" s="1">
         <v>2021</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>3522</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -27894,7 +30216,9 @@
       <c r="D8" s="1">
         <v>2021</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>3523</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -27909,7 +30233,9 @@
       <c r="D9" s="1">
         <v>2019</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>3524</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -27924,7 +30250,9 @@
       <c r="D10" s="1">
         <v>2021</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>3525</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -27939,7 +30267,9 @@
       <c r="D11" s="1">
         <v>2019</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>3526</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -27954,7 +30284,9 @@
       <c r="D12" s="1">
         <v>2021</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>3527</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -27969,7 +30301,9 @@
       <c r="D13" s="1">
         <v>2021</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>3528</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -27984,7 +30318,9 @@
       <c r="D14" s="1">
         <v>2020</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>3529</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>